<commit_message>
Updated text.xlsx files. Made changes in PrintTreeRecursive() function to be more readable in Main class. Slight modifications in Main class.
</commit_message>
<xml_diff>
--- a/src/main/java/Main/test.xlsx
+++ b/src/main/java/Main/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="101">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Ömer</t>
   </si>
   <si>
-    <t xml:space="preserve">Eda</t>
+    <t xml:space="preserve">Eda Kara</t>
   </si>
   <si>
     <t xml:space="preserve">A(+)</t>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">Öğretmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eda Kara</t>
   </si>
   <si>
     <t xml:space="preserve">Furkan</t>
@@ -442,16 +439,16 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="12.57"/>
   </cols>
@@ -972,11 +969,11 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
@@ -1116,7 +1113,7 @@
         <v>34808</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>29</v>
@@ -1226,7 +1223,7 @@
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
@@ -1283,7 +1280,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>36</v>
@@ -1295,16 +1292,16 @@
         <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
@@ -1328,13 +1325,13 @@
         <v>16595</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>39</v>
@@ -1346,7 +1343,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>28</v>
@@ -1357,22 +1354,22 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>23867</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>39</v>
@@ -1395,28 +1392,28 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24872</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
@@ -1433,7 +1430,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>36</v>
@@ -1442,19 +1439,19 @@
         <v>25852</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>19</v>
@@ -1469,22 +1466,22 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>32457</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>56</v>
@@ -1507,22 +1504,22 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>33094</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>39</v>
@@ -1543,28 +1540,28 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>32875</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
@@ -1579,28 +1576,28 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>33641</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -1621,22 +1618,22 @@
         <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>19</v>
@@ -1685,20 +1682,20 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>42469</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>46</v>
@@ -1717,20 +1714,20 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>43</v>
@@ -1749,20 +1746,20 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>43018</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>56</v>
@@ -1784,17 +1781,17 @@
         <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>41737</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>43</v>
@@ -1815,20 +1812,20 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>39</v>
@@ -1847,20 +1844,20 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>41199</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
@@ -1894,11 +1891,11 @@
   </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.7"/>
@@ -1955,28 +1952,28 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>16985</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>19</v>
@@ -1991,16 +1988,16 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>17924</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -2012,13 +2009,13 @@
         <v>56</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>28</v>
@@ -2029,28 +2026,28 @@
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>31695</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>19</v>
@@ -2065,20 +2062,20 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>41199</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -2099,20 +2096,20 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>34493</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>39</v>
@@ -2121,7 +2118,7 @@
         <v>57</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>28</v>
@@ -2135,14 +2132,14 @@
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>41733</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Implemented spouseID data handler in Family class. Updated excel files to be compatible with spouseID data handler system.
</commit_message>
<xml_diff>
--- a/src/main/java/Main/test.xlsx
+++ b/src/main/java/Main/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="114">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Kaya</t>
   </si>
   <si>
-    <t xml:space="preserve">Sena Kaya</t>
+    <t xml:space="preserve">2 Sena Kaya</t>
   </si>
   <si>
     <t xml:space="preserve">Ayşe</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Sena</t>
   </si>
   <si>
-    <t xml:space="preserve">Emin Kaya</t>
+    <t xml:space="preserve">1 Emin Kaya</t>
   </si>
   <si>
     <t xml:space="preserve">Hatice</t>
@@ -118,73 +118,79 @@
     <t xml:space="preserve">Demir</t>
   </si>
   <si>
-    <t xml:space="preserve">Uğur Demir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeynep  Kılıç</t>
+    <t xml:space="preserve">14 Uğur Demir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 Zeynep  Kılıç</t>
   </si>
   <si>
     <t xml:space="preserve">Mustafa</t>
   </si>
   <si>
+    <t xml:space="preserve">38 Elif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Çelik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Ahmet Çelik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uğur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB(+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mühendis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ömer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 Eda Kara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doktor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeynep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0(+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bekar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Öğrenci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alper</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elif</t>
   </si>
   <si>
-    <t xml:space="preserve">Defne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Çelik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmet Çelik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uğur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB(+)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mühendis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ömer</t>
+    <t xml:space="preserve">İrem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmet</t>
   </si>
   <si>
     <t xml:space="preserve">Eda Kara</t>
   </si>
   <si>
-    <t xml:space="preserve">A(+)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doktor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeynep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0(+)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bekar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Öğrenci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">İrem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nazlı Kaya</t>
+    <t xml:space="preserve">3 Nazlı Kaya</t>
   </si>
   <si>
     <t xml:space="preserve">Fatma</t>
@@ -202,6 +208,9 @@
     <t xml:space="preserve">Furkan</t>
   </si>
   <si>
+    <t xml:space="preserve">16 Zeynep</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feride</t>
   </si>
   <si>
@@ -211,6 +220,9 @@
     <t xml:space="preserve">Terzi</t>
   </si>
   <si>
+    <t xml:space="preserve">15 Furkan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hayriye</t>
   </si>
   <si>
@@ -226,72 +238,90 @@
     <t xml:space="preserve">Kurt</t>
   </si>
   <si>
+    <t xml:space="preserve">40 Faruk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gül</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Özkan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 Hasan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhasebeci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bekir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42 Kübra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aslan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 Mahmut Aslan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Faruk</t>
   </si>
   <si>
-    <t xml:space="preserve">Gül</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Özkan</t>
+    <t xml:space="preserve">43 Esra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orhan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 Feride</t>
   </si>
   <si>
     <t xml:space="preserve">Hasan</t>
   </si>
   <si>
-    <t xml:space="preserve">Muhasebeci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bekir</t>
+    <t xml:space="preserve">Necmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 Gökçe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/27/1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Defne</t>
   </si>
   <si>
     <t xml:space="preserve">Kübra</t>
   </si>
   <si>
-    <t xml:space="preserve">Semra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aslan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mahmut Aslan</t>
+    <t xml:space="preserve">Avukat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yusuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gökçe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/29/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merve</t>
   </si>
   <si>
     <t xml:space="preserve">Esra</t>
   </si>
   <si>
-    <t xml:space="preserve">Orhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necmi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gökçe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/27/1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avukat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yusuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/29/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merve</t>
-  </si>
-  <si>
     <t xml:space="preserve">Almila</t>
   </si>
   <si>
-    <t xml:space="preserve">02/14/2016</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yılmaz</t>
   </si>
   <si>
@@ -301,22 +331,31 @@
     <t xml:space="preserve">Yakup</t>
   </si>
   <si>
+    <t xml:space="preserve">32 Funda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazi-fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">İşçi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Funda</t>
   </si>
   <si>
-    <t xml:space="preserve">Nazi-fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">İşçi</t>
+    <t xml:space="preserve">31 Yakup</t>
   </si>
   <si>
     <t xml:space="preserve">Fabrikatör</t>
   </si>
   <si>
     <t xml:space="preserve">Erdoğan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Semra</t>
   </si>
   <si>
     <t xml:space="preserve">Yıldız</t>
@@ -332,9 +371,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -402,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -412,6 +452,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,10 +483,10 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.71"/>
@@ -866,7 +910,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>33</v>
@@ -890,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -903,7 +947,7 @@
         <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>43</v>
@@ -934,7 +978,7 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>41</v>
@@ -969,11 +1013,11 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
@@ -1039,19 +1083,19 @@
         <v>24657</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
@@ -1140,7 +1184,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>36</v>
@@ -1153,7 +1197,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>43</v>
@@ -1184,7 +1228,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>41</v>
@@ -1220,15 +1264,15 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.85"/>
@@ -1280,7 +1324,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>36</v>
@@ -1289,19 +1333,19 @@
         <v>14977</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
@@ -1325,13 +1369,13 @@
         <v>16595</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>39</v>
@@ -1343,7 +1387,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>28</v>
@@ -1354,22 +1398,22 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>23867</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>39</v>
@@ -1392,28 +1436,28 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24872</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
@@ -1430,7 +1474,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>36</v>
@@ -1439,19 +1483,19 @@
         <v>25852</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>19</v>
@@ -1466,25 +1510,25 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>32457</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>26</v>
@@ -1504,22 +1548,22 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>33094</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>39</v>
@@ -1540,28 +1584,28 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>32875</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
@@ -1576,28 +1620,28 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>33641</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -1612,28 +1656,28 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>19</v>
@@ -1648,7 +1692,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
@@ -1661,7 +1705,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>43</v>
@@ -1682,20 +1726,20 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>42469</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>46</v>
@@ -1714,20 +1758,20 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>43</v>
@@ -1746,23 +1790,23 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>43018</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
@@ -1778,20 +1822,20 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>41737</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>43</v>
@@ -1807,25 +1851,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>42414</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>39</v>
@@ -1844,20 +1888,20 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>41199</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
@@ -1891,11 +1935,11 @@
   </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.7"/>
@@ -1951,34 +1995,34 @@
       <c r="A2" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>75</v>
+      <c r="B2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>16985</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3"/>
+      <c r="I2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="4"/>
       <c r="L2" s="0" t="s">
         <v>20</v>
       </c>
@@ -1987,35 +2031,35 @@
       <c r="A3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>75</v>
+      <c r="B3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>17924</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>97</v>
+      <c r="H3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>28</v>
@@ -2026,28 +2070,28 @@
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>31695</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>19</v>
@@ -2062,20 +2106,20 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>41199</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -2096,29 +2140,29 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>34493</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>28</v>
@@ -2129,20 +2173,20 @@
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>41733</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>17</v>

</xml_diff>